<commit_message>
some minor changes to make nicer labels on the figures.
</commit_message>
<xml_diff>
--- a/sample_sheets/pbmc_samples_202102.xlsx
+++ b/sample_sheets/pbmc_samples_202102.xlsx
@@ -24,11 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="153">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
   <si>
+    <t xml:space="preserve">figure label</t>
+  </si>
+  <si>
     <t xml:space="preserve">experiment_name</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
     <t xml:space="preserve">HPGL0630</t>
   </si>
   <si>
+    <t xml:space="preserve">uninf</t>
+  </si>
+  <si>
     <t xml:space="preserve">infection</t>
   </si>
   <si>
@@ -164,9 +170,6 @@
     <t xml:space="preserve">Healthy-Uninfected</t>
   </si>
   <si>
-    <t xml:space="preserve">uninf</t>
-  </si>
-  <si>
     <t xml:space="preserve">d108</t>
   </si>
   <si>
@@ -215,6 +218,9 @@
     <t xml:space="preserve">HPGL0631</t>
   </si>
   <si>
+    <t xml:space="preserve">ch5430</t>
+  </si>
+  <si>
     <t xml:space="preserve">PG108 PBMC 5430-1</t>
   </si>
   <si>
@@ -248,6 +254,9 @@
     <t xml:space="preserve">HPGL0632</t>
   </si>
   <si>
+    <t xml:space="preserve">ch5397</t>
+  </si>
+  <si>
     <t xml:space="preserve">PG108 PBMC 5397-1</t>
   </si>
   <si>
@@ -263,6 +272,9 @@
     <t xml:space="preserve">HPGL0633</t>
   </si>
   <si>
+    <t xml:space="preserve">ch2504</t>
+  </si>
+  <si>
     <t xml:space="preserve">PG108 PBMC 2504-1</t>
   </si>
   <si>
@@ -278,6 +290,9 @@
     <t xml:space="preserve">HPGL0634</t>
   </si>
   <si>
+    <t xml:space="preserve">sh2272</t>
+  </si>
+  <si>
     <t xml:space="preserve">PG108 PBMC 2272-1</t>
   </si>
   <si>
@@ -302,6 +317,9 @@
     <t xml:space="preserve">HPGL0635</t>
   </si>
   <si>
+    <t xml:space="preserve">sh1022</t>
+  </si>
+  <si>
     <t xml:space="preserve">PG108 PBMC 1022-1</t>
   </si>
   <si>
@@ -315,6 +333,9 @@
   </si>
   <si>
     <t xml:space="preserve">HPGL0636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh2189</t>
   </si>
   <si>
     <t xml:space="preserve">PG108 PBMC 2189-1</t>
@@ -563,39 +584,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AP23"/>
+  <dimension ref="A1:AQ23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="216" zoomScaleNormal="216" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK3" activeCellId="0" sqref="AK3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="28.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="14.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="28.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="17" style="1" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="68.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="29.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="38" style="1" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="1015" style="0" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1020" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1021" style="0" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="28.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="36" min="18" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="68.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="29.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="39" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1016" style="0" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="0" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +727,7 @@
       <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
       <c r="AL1" s="1" t="s">
@@ -724,26 +744,29 @@
       </c>
       <c r="AP1" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>48</v>
@@ -755,16 +778,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>52</v>
@@ -772,17 +795,17 @@
       <c r="O2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="2"/>
       <c r="U2" s="2" t="s">
         <v>56</v>
       </c>
@@ -792,113 +815,116 @@
       <c r="W2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="2"/>
+      <c r="X2" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="2" t="n">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2" t="n">
         <v>269</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE2" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
-      <c r="AH2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI2" s="2" t="str">
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" s="2" t="str">
         <f aca="false">LOWER(A2)</f>
         <v>hpgl0630</v>
       </c>
-      <c r="AJ2" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI2,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK2" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ2,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0630/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL2" s="0" t="n">
+      <c r="AL2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM2" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM2" s="1" t="n">
+      <c r="AN2" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN2" s="1" t="n">
+      <c r="AO2" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO2" s="1" t="n">
+      <c r="AP2" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP2" s="1" t="n">
+      <c r="AQ2" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
         <v>56</v>
       </c>
@@ -909,118 +935,121 @@
         <v>58</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA3" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB3" s="2" t="n">
         <v>271</v>
       </c>
-      <c r="AB3" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE3" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI3" s="2" t="str">
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ3" s="2" t="str">
         <f aca="false">LOWER(A3)</f>
         <v>hpgl0631</v>
       </c>
-      <c r="AJ3" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI3,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK3" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ3,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0631/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL3" s="0" t="n">
+      <c r="AL3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM3" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM3" s="1" t="n">
+      <c r="AN3" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN3" s="1" t="n">
+      <c r="AO3" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO3" s="1" t="n">
+      <c r="AP3" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP3" s="1" t="n">
+      <c r="AQ3" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q4" s="2"/>
       <c r="R4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="2"/>
       <c r="U4" s="2" t="s">
         <v>56</v>
       </c>
@@ -1031,118 +1060,121 @@
         <v>58</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA4" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB4" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="AB4" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC4" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE4" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF4" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
-      <c r="AH4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI4" s="2" t="str">
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ4" s="2" t="str">
         <f aca="false">LOWER(A4)</f>
         <v>hpgl0632</v>
       </c>
-      <c r="AJ4" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI4,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK4" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ4,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0632/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL4" s="0" t="n">
+      <c r="AL4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM4" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM4" s="1" t="n">
+      <c r="AN4" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN4" s="1" t="n">
+      <c r="AO4" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO4" s="1" t="n">
+      <c r="AP4" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP4" s="1" t="n">
+      <c r="AQ4" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q5" s="2"/>
       <c r="R5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="2"/>
       <c r="U5" s="2" t="s">
         <v>56</v>
       </c>
@@ -1153,118 +1185,121 @@
         <v>58</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA5" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB5" s="2" t="n">
         <v>176</v>
       </c>
-      <c r="AB5" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE5" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF5" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
-      <c r="AH5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI5" s="2" t="str">
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ5" s="2" t="str">
         <f aca="false">LOWER(A5)</f>
         <v>hpgl0633</v>
       </c>
-      <c r="AJ5" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI5,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK5" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ5,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0633/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL5" s="0" t="n">
+      <c r="AL5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM5" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM5" s="1" t="n">
+      <c r="AN5" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN5" s="1" t="n">
+      <c r="AO5" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO5" s="1" t="n">
+      <c r="AP5" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP5" s="1" t="n">
+      <c r="AQ5" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T6" s="2"/>
       <c r="U6" s="2" t="s">
         <v>56</v>
       </c>
@@ -1275,118 +1310,121 @@
         <v>58</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA6" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB6" s="2" t="n">
         <v>243</v>
       </c>
-      <c r="AB6" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC6" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE6" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
-      <c r="AH6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI6" s="2" t="str">
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ6" s="2" t="str">
         <f aca="false">LOWER(A6)</f>
         <v>hpgl0634</v>
       </c>
-      <c r="AJ6" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI6,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK6" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ6,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0634/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL6" s="0" t="n">
+      <c r="AL6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM6" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM6" s="1" t="n">
+      <c r="AN6" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN6" s="1" t="n">
+      <c r="AO6" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO6" s="1" t="n">
+      <c r="AP6" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP6" s="1" t="n">
+      <c r="AQ6" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q7" s="2"/>
       <c r="R7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
         <v>56</v>
       </c>
@@ -1397,118 +1435,121 @@
         <v>58</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA7" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB7" s="2" t="n">
         <v>284</v>
       </c>
-      <c r="AB7" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC7" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE7" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
-      <c r="AH7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI7" s="2" t="str">
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ7" s="2" t="str">
         <f aca="false">LOWER(A7)</f>
         <v>hpgl0635</v>
       </c>
-      <c r="AJ7" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI7,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK7" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ7,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0635/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL7" s="0" t="n">
+      <c r="AL7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM7" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM7" s="1" t="n">
+      <c r="AN7" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN7" s="1" t="n">
+      <c r="AO7" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO7" s="1" t="n">
+      <c r="AP7" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP7" s="1" t="n">
+      <c r="AQ7" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q8" s="2"/>
       <c r="R8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" s="2"/>
       <c r="U8" s="2" t="s">
         <v>56</v>
       </c>
@@ -1519,100 +1560,103 @@
         <v>58</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA8" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB8" s="2" t="n">
         <v>306</v>
       </c>
-      <c r="AB8" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC8" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE8" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF8" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
-      <c r="AH8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI8" s="2" t="str">
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ8" s="2" t="str">
         <f aca="false">LOWER(A8)</f>
         <v>hpgl0636</v>
       </c>
-      <c r="AJ8" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI8,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK8" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ8,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0636/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AL8" s="0" t="n">
+      <c r="AL8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM8" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM8" s="1" t="n">
+      <c r="AN8" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN8" s="1" t="n">
+      <c r="AO8" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO8" s="1" t="n">
+      <c r="AP8" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP8" s="1" t="n">
+      <c r="AQ8" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>52</v>
@@ -1620,17 +1664,17 @@
       <c r="O9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="2"/>
       <c r="U9" s="2" t="s">
         <v>56</v>
       </c>
@@ -1640,113 +1684,116 @@
       <c r="W9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="X9" s="2"/>
+      <c r="X9" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="2" t="n">
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2" t="n">
         <v>149</v>
       </c>
-      <c r="AB9" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC9" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE9" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
-      <c r="AH9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI9" s="2" t="str">
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ9" s="2" t="str">
         <f aca="false">LOWER(A9)</f>
         <v>hpgl0650</v>
       </c>
-      <c r="AJ9" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI9,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK9" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ9,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0650/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL9" s="0" t="n">
+      <c r="AL9" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM9" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM9" s="1" t="n">
+      <c r="AN9" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN9" s="1" t="n">
+      <c r="AO9" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO9" s="1" t="n">
+      <c r="AP9" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP9" s="1" t="n">
+      <c r="AQ9" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q10" s="2"/>
       <c r="R10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T10" s="2"/>
       <c r="U10" s="2" t="s">
         <v>56</v>
       </c>
@@ -1757,118 +1804,121 @@
         <v>58</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA10" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB10" s="2" t="n">
         <v>96</v>
       </c>
-      <c r="AB10" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC10" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE10" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF10" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
-      <c r="AH10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI10" s="2" t="str">
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ10" s="2" t="str">
         <f aca="false">LOWER(A10)</f>
         <v>hpgl0651</v>
       </c>
-      <c r="AJ10" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI10,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK10" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ10,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0651/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL10" s="0" t="n">
+      <c r="AL10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM10" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM10" s="1" t="n">
+      <c r="AN10" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN10" s="1" t="n">
+      <c r="AO10" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO10" s="1" t="n">
+      <c r="AP10" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP10" s="1" t="n">
+      <c r="AQ10" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q11" s="2"/>
       <c r="R11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T11" s="2"/>
       <c r="U11" s="2" t="s">
         <v>56</v>
       </c>
@@ -1879,118 +1929,121 @@
         <v>58</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA11" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB11" s="2" t="n">
         <v>115</v>
       </c>
-      <c r="AB11" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC11" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE11" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
-      <c r="AH11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI11" s="2" t="str">
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ11" s="2" t="str">
         <f aca="false">LOWER(A11)</f>
         <v>hpgl0652</v>
       </c>
-      <c r="AJ11" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI11,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK11" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ11,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0652/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL11" s="0" t="n">
+      <c r="AL11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM11" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM11" s="1" t="n">
+      <c r="AN11" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN11" s="1" t="n">
+      <c r="AO11" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO11" s="1" t="n">
+      <c r="AP11" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP11" s="1" t="n">
+      <c r="AQ11" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q12" s="2"/>
       <c r="R12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T12" s="2"/>
       <c r="U12" s="2" t="s">
         <v>56</v>
       </c>
@@ -2001,118 +2054,121 @@
         <v>58</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA12" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB12" s="2" t="n">
         <v>233</v>
       </c>
-      <c r="AB12" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC12" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE12" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
-      <c r="AH12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI12" s="2" t="str">
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ12" s="2" t="str">
         <f aca="false">LOWER(A12)</f>
         <v>hpgl0653</v>
       </c>
-      <c r="AJ12" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI12,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK12" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ12,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0653/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL12" s="0" t="n">
+      <c r="AL12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM12" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM12" s="1" t="n">
+      <c r="AN12" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN12" s="1" t="n">
+      <c r="AO12" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO12" s="1" t="n">
+      <c r="AP12" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP12" s="1" t="n">
+      <c r="AQ12" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q13" s="2"/>
       <c r="R13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T13" s="2"/>
       <c r="U13" s="2" t="s">
         <v>56</v>
       </c>
@@ -2123,118 +2179,121 @@
         <v>58</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA13" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB13" s="2" t="n">
         <v>249</v>
       </c>
-      <c r="AB13" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC13" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE13" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF13" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI13" s="2" t="str">
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ13" s="2" t="str">
         <f aca="false">LOWER(A13)</f>
         <v>hpgl0654</v>
       </c>
-      <c r="AJ13" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI13,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK13" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ13,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0654/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK13" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AL13" s="0" t="n">
+      <c r="AL13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AM13" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM13" s="1" t="n">
+      <c r="AN13" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN13" s="1" t="n">
+      <c r="AO13" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO13" s="1" t="n">
+      <c r="AP13" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP13" s="1" t="n">
+      <c r="AQ13" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q14" s="2"/>
       <c r="R14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T14" s="2"/>
       <c r="U14" s="2" t="s">
         <v>56</v>
       </c>
@@ -2245,118 +2304,121 @@
         <v>58</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA14" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB14" s="2" t="n">
         <v>274</v>
       </c>
-      <c r="AB14" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE14" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF14" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
-      <c r="AH14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI14" s="2" t="str">
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ14" s="2" t="str">
         <f aca="false">LOWER(A14)</f>
         <v>hpgl0655</v>
       </c>
-      <c r="AJ14" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI14,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK14" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ14,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0655/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AL14" s="0" t="n">
+      <c r="AL14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM14" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM14" s="1" t="n">
+      <c r="AN14" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN14" s="1" t="n">
+      <c r="AO14" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO14" s="1" t="n">
+      <c r="AP14" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP14" s="1" t="n">
+      <c r="AQ14" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q15" s="2"/>
       <c r="R15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T15" s="2"/>
       <c r="U15" s="2" t="s">
         <v>56</v>
       </c>
@@ -2367,100 +2429,103 @@
         <v>58</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA15" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB15" s="2" t="n">
         <v>238</v>
       </c>
-      <c r="AB15" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC15" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE15" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF15" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
-      <c r="AH15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI15" s="2" t="str">
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ15" s="2" t="str">
         <f aca="false">LOWER(A15)</f>
         <v>hpgl0656</v>
       </c>
-      <c r="AJ15" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI15,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK15" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ15,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0656/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AL15" s="0" t="n">
+      <c r="AL15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM15" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM15" s="1" t="n">
+      <c r="AN15" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN15" s="1" t="n">
+      <c r="AO15" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO15" s="1" t="n">
+      <c r="AP15" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP15" s="1" t="n">
+      <c r="AQ15" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>52</v>
@@ -2468,17 +2533,17 @@
       <c r="O16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q16" s="2"/>
       <c r="R16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T16" s="2"/>
       <c r="U16" s="2" t="s">
         <v>56</v>
       </c>
@@ -2488,113 +2553,116 @@
       <c r="W16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="X16" s="2"/>
+      <c r="X16" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
-      <c r="AA16" s="2" t="n">
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2" t="n">
         <v>157</v>
       </c>
-      <c r="AB16" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC16" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE16" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
-      <c r="AH16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI16" s="2" t="str">
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ16" s="2" t="str">
         <f aca="false">LOWER(A16)</f>
         <v>hpgl0657</v>
       </c>
-      <c r="AJ16" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI16,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK16" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ16,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0657/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK16" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL16" s="0" t="n">
+      <c r="AL16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM16" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM16" s="1" t="n">
+      <c r="AN16" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN16" s="1" t="n">
+      <c r="AO16" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO16" s="1" t="n">
+      <c r="AP16" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP16" s="1" t="n">
+      <c r="AQ16" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>64</v>
+        <v>135</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q17" s="2"/>
       <c r="R17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T17" s="2"/>
       <c r="U17" s="2" t="s">
         <v>56</v>
       </c>
@@ -2605,118 +2673,121 @@
         <v>58</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA17" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB17" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="AB17" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC17" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE17" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF17" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
-      <c r="AH17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI17" s="2" t="str">
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ17" s="2" t="str">
         <f aca="false">LOWER(A17)</f>
         <v>hpgl0658</v>
       </c>
-      <c r="AJ17" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI17,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK17" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ17,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0658/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK17" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL17" s="0" t="n">
+      <c r="AL17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM17" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM17" s="1" t="n">
+      <c r="AN17" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN17" s="1" t="n">
+      <c r="AO17" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO17" s="1" t="n">
+      <c r="AP17" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP17" s="1" t="n">
+      <c r="AQ17" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q18" s="2"/>
       <c r="R18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T18" s="2"/>
       <c r="U18" s="2" t="s">
         <v>56</v>
       </c>
@@ -2727,118 +2798,121 @@
         <v>58</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA18" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB18" s="2" t="n">
         <v>225</v>
       </c>
-      <c r="AB18" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC18" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE18" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF18" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
-      <c r="AH18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI18" s="2" t="str">
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ18" s="2" t="str">
         <f aca="false">LOWER(A18)</f>
         <v>hpgl0659</v>
       </c>
-      <c r="AJ18" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI18,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK18" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ18,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0659/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AL18" s="0" t="n">
+      <c r="AL18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM18" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM18" s="1" t="n">
+      <c r="AN18" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN18" s="1" t="n">
+      <c r="AO18" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO18" s="1" t="n">
+      <c r="AP18" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP18" s="1" t="n">
+      <c r="AQ18" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="I19" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q19" s="2"/>
       <c r="R19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T19" s="2"/>
       <c r="U19" s="2" t="s">
         <v>56</v>
       </c>
@@ -2849,118 +2923,121 @@
         <v>58</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA19" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB19" s="2" t="n">
         <v>248</v>
       </c>
-      <c r="AB19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC19" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE19" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF19" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI19" s="2" t="str">
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ19" s="2" t="str">
         <f aca="false">LOWER(A19)</f>
         <v>hpgl0660</v>
       </c>
-      <c r="AJ19" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI19,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK19" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ19,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0660/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK19" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AL19" s="0" t="n">
+      <c r="AL19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AM19" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM19" s="1" t="n">
+      <c r="AN19" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN19" s="1" t="n">
+      <c r="AO19" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO19" s="1" t="n">
+      <c r="AP19" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP19" s="1" t="n">
+      <c r="AQ19" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q20" s="2"/>
       <c r="R20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" s="2"/>
       <c r="U20" s="2" t="s">
         <v>56</v>
       </c>
@@ -2971,118 +3048,121 @@
         <v>58</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA20" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB20" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="AB20" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC20" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE20" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF20" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
-      <c r="AH20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI20" s="2" t="str">
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ20" s="2" t="str">
         <f aca="false">LOWER(A20)</f>
         <v>hpgl0661</v>
       </c>
-      <c r="AJ20" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI20,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK20" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ20,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0661/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK20" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL20" s="0" t="n">
+      <c r="AL20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM20" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM20" s="1" t="n">
+      <c r="AN20" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN20" s="1" t="n">
+      <c r="AO20" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO20" s="1" t="n">
+      <c r="AP20" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP20" s="1" t="n">
+      <c r="AQ20" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="I21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2" t="s">
+      <c r="P21" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q21" s="2"/>
       <c r="R21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T21" s="2"/>
       <c r="U21" s="2" t="s">
         <v>56</v>
       </c>
@@ -3093,118 +3173,121 @@
         <v>58</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA21" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB21" s="2" t="n">
         <v>145</v>
       </c>
-      <c r="AB21" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC21" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE21" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF21" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
-      <c r="AH21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI21" s="2" t="str">
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ21" s="2" t="str">
         <f aca="false">LOWER(A21)</f>
         <v>hpgl0662</v>
       </c>
-      <c r="AJ21" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI21,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK21" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ21,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0662/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK21" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AL21" s="0" t="n">
+      <c r="AL21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM21" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM21" s="1" t="n">
+      <c r="AN21" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN21" s="1" t="n">
+      <c r="AO21" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO21" s="1" t="n">
+      <c r="AP21" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP21" s="1" t="n">
+      <c r="AQ21" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P22" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="Q22" s="2"/>
       <c r="R22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="S22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T22" s="2"/>
       <c r="U22" s="2" t="s">
         <v>56</v>
       </c>
@@ -3215,58 +3298,61 @@
         <v>58</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA22" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB22" s="2" t="n">
         <v>305</v>
       </c>
-      <c r="AB22" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AC22" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE22" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AE22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF22" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
-      <c r="AH22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI22" s="2" t="str">
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ22" s="2" t="str">
         <f aca="false">LOWER(A22)</f>
         <v>hpgl0663</v>
       </c>
-      <c r="AJ22" s="2" t="str">
-        <f aca="false">CONCATENATE("preprocessing/",AI22,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
+      <c r="AK22" s="2" t="str">
+        <f aca="false">CONCATENATE("preprocessing/",AJ22,"/outputs/tophat_hsapiens/accepted_paired.count.xz")</f>
         <v>preprocessing/hpgl0663/outputs/tophat_hsapiens/accepted_paired.count.xz</v>
       </c>
-      <c r="AK22" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AL22" s="0" t="n">
+      <c r="AL22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM22" s="0" t="n">
         <v>76.4</v>
       </c>
-      <c r="AM22" s="1" t="n">
+      <c r="AN22" s="1" t="n">
         <v>19.4</v>
       </c>
-      <c r="AN22" s="1" t="n">
+      <c r="AO22" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="AO22" s="1" t="n">
+      <c r="AP22" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AP22" s="1" t="n">
+      <c r="AQ22" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -3276,10 +3362,10 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -3309,6 +3395,7 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>